<commit_message>
Gerbers and Schematic Completed for Prototype
The layout was modified to accomodate non-oval drills and drill files
were merged.  All manufacturers, part numbers and datasheet fields have
been completed in the schematic.
</commit_message>
<xml_diff>
--- a/MSGEQ7_Breakout_Board/MSGEQ7_Breakout_Board_BOM.xlsx
+++ b/MSGEQ7_Breakout_Board/MSGEQ7_Breakout_Board_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
   <si>
     <t>Index</t>
   </si>
@@ -164,13 +164,19 @@
     <t>Stereo Mini Jack</t>
   </si>
   <si>
-    <t>CUI Iinc</t>
-  </si>
-  <si>
-    <t>SJ1-352XNG</t>
-  </si>
-  <si>
     <t>3-pin Custom</t>
+  </si>
+  <si>
+    <t>SJ1-3523NG</t>
+  </si>
+  <si>
+    <t>CUI Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sullins Connector </t>
+  </si>
+  <si>
+    <t>PREC040SAAN-RC</t>
   </si>
 </sst>
 </file>
@@ -914,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1153,11 +1159,19 @@
       <c r="D7" t="s">
         <v>45</v>
       </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="N7" s="8"/>
       <c r="O7" t="s">
         <v>46</v>
@@ -1178,7 +1192,7 @@
         <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>
@@ -1191,7 +1205,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O8" t="s">
         <v>12</v>
@@ -1339,11 +1353,12 @@
     <hyperlink ref="M5" r:id="rId4"/>
     <hyperlink ref="M6" r:id="rId5"/>
     <hyperlink ref="M8" r:id="rId6"/>
+    <hyperlink ref="M7" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
All Design Files Updated to KiCad v4.0.0_RC1
</commit_message>
<xml_diff>
--- a/MSGEQ7_Breakout_Board/MSGEQ7_Breakout_Board_BOM.xlsx
+++ b/MSGEQ7_Breakout_Board/MSGEQ7_Breakout_Board_BOM.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="0" windowWidth="7200" windowHeight="10650"/>
+    <workbookView xWindow="7365" yWindow="0" windowWidth="7200" windowHeight="10650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MSGEQ7 Breakout Board BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Order Work Sheet" sheetId="5" r:id="rId2"/>
-    <sheet name="PCB Fabrication" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
   <si>
     <t>Index</t>
   </si>
@@ -108,9 +107,6 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>K103K15X7RF53L2</t>
-  </si>
-  <si>
     <t>PTH 2.5mm Spacing</t>
   </si>
   <si>
@@ -132,9 +128,6 @@
     <t>PTH 6mm body / .55mm lead dia.</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>Input Resistor 22K</t>
   </si>
   <si>
@@ -156,9 +149,6 @@
     <t>6 Pin Header</t>
   </si>
   <si>
-    <t>SIL-6</t>
-  </si>
-  <si>
     <t>Audio In Jack</t>
   </si>
   <si>
@@ -183,9 +173,6 @@
     <t>0.1" Spaced Header</t>
   </si>
   <si>
-    <t>BC1078CT-ND</t>
-  </si>
-  <si>
     <t>BC1007CT-ND</t>
   </si>
   <si>
@@ -213,81 +200,9 @@
     <t>Parts Cost Per Board:</t>
   </si>
   <si>
-    <t xml:space="preserve">Board Dimension </t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Board Area</t>
-  </si>
-  <si>
-    <t>XY</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>sqin</t>
-  </si>
-  <si>
-    <t>Cost Per sqin</t>
-  </si>
-  <si>
-    <t>Min. sqin</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Order Multiple</t>
-  </si>
-  <si>
-    <t>Boards: sqin min.</t>
-  </si>
-  <si>
-    <t>Boards: mult. min.</t>
-  </si>
-  <si>
-    <t>Qty: 90</t>
-  </si>
-  <si>
-    <t>Prototype Service</t>
-  </si>
-  <si>
-    <t>Medium Run Service</t>
-  </si>
-  <si>
-    <t>Qty: 100</t>
-  </si>
-  <si>
-    <t>Qty: 80</t>
-  </si>
-  <si>
-    <t>Qty: 70</t>
-  </si>
-  <si>
-    <t>Qty: 60</t>
-  </si>
-  <si>
-    <t>Qty: 50</t>
-  </si>
-  <si>
-    <t>Qty: 40</t>
-  </si>
-  <si>
-    <t>Qty: 30</t>
-  </si>
-  <si>
-    <t>Qty: 20</t>
-  </si>
-  <si>
-    <t>Qty: 10</t>
-  </si>
-  <si>
     <t>PREC005SAAN-RC</t>
   </si>
   <si>
@@ -297,10 +212,37 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>490-8814-ND</t>
-  </si>
-  <si>
-    <t>RDER71H104K0K1H03B</t>
+    <t>PTH 5.0mm Spacing</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>PTH_RESISTOR</t>
+  </si>
+  <si>
+    <t>PIN_ARRAY_5x1</t>
+  </si>
+  <si>
+    <t>x / x</t>
+  </si>
+  <si>
+    <t>PCB Fabrication</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>OSH Park</t>
+  </si>
+  <si>
+    <t>RDER71H104K0M1H03A</t>
+  </si>
+  <si>
+    <t>490-9144-1-ND</t>
   </si>
 </sst>
 </file>
@@ -313,7 +255,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,14 +279,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,7 +340,7 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,15 +364,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,16 +376,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1054,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1101,16 +1026,16 @@
       <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1140,39 +1065,41 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="I2" s="3">
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J2" s="3">
-        <v>0.17699999999999999</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="K2" s="3">
-        <v>0.17699999999999999</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="L2" s="3">
-        <v>0.1003</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1">
@@ -1182,22 +1109,22 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I3" s="3">
         <v>0.34</v>
@@ -1215,12 +1142,14 @@
         <v>4</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1">
@@ -1230,22 +1159,22 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
         <v>53</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
       </c>
       <c r="I4" s="3">
         <v>0.1</v>
@@ -1263,12 +1192,14 @@
         <v>4</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P4" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1">
@@ -1278,22 +1209,22 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I5" s="3">
         <v>0.1</v>
@@ -1311,12 +1242,14 @@
         <v>4</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1">
@@ -1326,22 +1259,22 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I6" s="2">
         <v>3.96</v>
@@ -1359,12 +1292,14 @@
         <v>4</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1">
@@ -1377,42 +1312,44 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="11">
+        <v>63</v>
+      </c>
+      <c r="I7" s="10">
         <v>0.16</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>0.14599999999999999</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>0.14599999999999999</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>0.1202</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>46</v>
-      </c>
-      <c r="P7" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="1">
@@ -1422,47 +1359,85 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
       <c r="H8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="11">
+        <v>58</v>
+      </c>
+      <c r="I8" s="10">
         <v>1.04</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <v>0.80800000000000005</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <v>0.80800000000000005</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <v>0.61650000000000005</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="O8" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="3">
+        <v>2.93</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.93</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2.93</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1.29</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="6"/>
       <c r="P9" s="1"/>
@@ -1489,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15"/>
@@ -1501,7 +1476,7 @@
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
@@ -1581,46 +1556,46 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1">
-        <v>53</v>
-      </c>
-      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K2" s="15">
+        <v>3</v>
+      </c>
+      <c r="K2" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="M2" s="3">
-        <v>0.31</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="N2" s="3">
-        <v>0.23100000000000001</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="O2" s="3">
-        <v>0.23100000000000001</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="P2" s="3">
-        <v>0.10780000000000001</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="Q2" s="3">
         <f>IF(K2=0,0,((LOOKUP(K2, {1,10,25,100}, M2:P2)) * K2))</f>
-        <v>12.243</v>
+        <v>0.84000000000000008</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1631,36 +1606,36 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>53</v>
-      </c>
-      <c r="J3" s="16">
+        <v>1</v>
+      </c>
+      <c r="J3" s="14">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K3" s="15">
+        <v>1</v>
+      </c>
+      <c r="K3" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M3" s="3">
         <v>0.34</v>
@@ -1676,7 +1651,7 @@
       </c>
       <c r="Q3" s="3">
         <f>IF(K3=0,0,((LOOKUP(K3, {1,10,25,100}, M3:P3)) * K3))</f>
-        <v>13.356</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1687,36 +1662,36 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14">
+        <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="13">
+        <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
         <v>53</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>53</v>
-      </c>
-      <c r="J4" s="16">
-        <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K4" s="15">
-        <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>57</v>
       </c>
       <c r="M4" s="3">
         <v>0.1</v>
@@ -1732,7 +1707,7 @@
       </c>
       <c r="Q4" s="3">
         <f>IF(K4=0,0,((LOOKUP(K4, {1,10,25,100}, M4:P4)) * K4))</f>
-        <v>2.8089999999999997</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1743,36 +1718,36 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1">
-        <v>53</v>
-      </c>
-      <c r="J5" s="16">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K5" s="15">
+        <v>2</v>
+      </c>
+      <c r="K5" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M5" s="3">
         <v>0.1</v>
@@ -1788,7 +1763,7 @@
       </c>
       <c r="Q5" s="3">
         <f>IF(K5=0,0,((LOOKUP(K5, {1,10,25,100}, M5:P5)) * K5))</f>
-        <v>2.8089999999999997</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1799,36 +1774,36 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>53</v>
-      </c>
-      <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K6" s="15">
+        <v>1</v>
+      </c>
+      <c r="K6" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M6" s="2">
         <v>3.96</v>
@@ -1844,7 +1819,7 @@
       </c>
       <c r="Q6" s="3">
         <f>IF(K6=0,0,((LOOKUP(K6, {1,10,25,100}, M6:P6)) * K6))</f>
-        <v>209.88</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1858,49 +1833,49 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="1">
-        <v>53</v>
-      </c>
-      <c r="J7" s="16">
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K7" s="15">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="11">
+        <v>56</v>
+      </c>
+      <c r="M7" s="10">
         <v>0.18</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="10">
         <v>0.157</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <v>0.157</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="10">
         <v>0.12959999999999999</v>
       </c>
       <c r="Q7" s="3">
         <f>IF(K7=0,0,((LOOKUP(K7, {1,10,25,100}, M7:P7)) * K7))</f>
-        <v>8.3209999999999997</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1911,239 +1886,239 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>53</v>
-      </c>
-      <c r="J8" s="16">
+        <v>1</v>
+      </c>
+      <c r="J8" s="14">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
-      </c>
-      <c r="K8" s="15">
+        <v>1</v>
+      </c>
+      <c r="K8" s="13">
         <f>Table13[[#This Row],[Qty / Assy]]*Table13[[#This Row],[Assy]]</f>
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="11">
+        <v>58</v>
+      </c>
+      <c r="M8" s="10">
         <v>1.04</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="10">
         <v>0.80800000000000005</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="10">
         <v>0.80800000000000005</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="10">
         <v>0.61650000000000005</v>
       </c>
       <c r="Q8" s="3">
         <f>IF(K8=0,0,((LOOKUP(K8, {1,10,25,100}, M8:P8)) * K8))</f>
-        <v>42.824000000000005</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="1:17" ht="17.25">
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q10" s="17">
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="15">
         <f>SUM(Q2:Q9)</f>
-        <v>292.24200000000002</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q12" s="19">
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="17">
         <f>Q10/I2</f>
-        <v>5.5140000000000002</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
+      <c r="K15" s="11"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-    </row>
-    <row r="17" spans="13:16">
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-    </row>
-    <row r="18" spans="13:16">
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-    </row>
-    <row r="19" spans="13:16">
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-    </row>
-    <row r="20" spans="13:16">
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="13:16">
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-    </row>
-    <row r="22" spans="13:16">
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-    </row>
-    <row r="23" spans="13:16">
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="12"/>
-    </row>
-    <row r="24" spans="13:16">
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="13:16">
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-    </row>
-    <row r="26" spans="13:16">
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-    </row>
-    <row r="27" spans="13:16">
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-    </row>
-    <row r="28" spans="13:16">
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-    </row>
-    <row r="29" spans="13:16">
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-    </row>
-    <row r="30" spans="13:16">
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-    </row>
-    <row r="31" spans="13:16">
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-    </row>
-    <row r="32" spans="13:16">
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
+      <c r="K16" s="11"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="11:16">
+      <c r="K17" s="11"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="11:16">
+      <c r="K18" s="11"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="11:16">
+      <c r="K19" s="11"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="11:16">
+      <c r="K20" s="11"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="11:16">
+      <c r="K21" s="11"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="11:16">
+      <c r="K22" s="11"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="11:16">
+      <c r="K23" s="11"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="11:16">
+      <c r="K24" s="11"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="11:16">
+      <c r="K25" s="11"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="11:16">
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+    </row>
+    <row r="27" spans="11:16">
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+    </row>
+    <row r="28" spans="11:16">
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+    </row>
+    <row r="29" spans="11:16">
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+    </row>
+    <row r="30" spans="11:16">
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+    </row>
+    <row r="31" spans="11:16">
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+    </row>
+    <row r="32" spans="11:16">
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
     </row>
     <row r="33" spans="13:16">
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
     </row>
     <row r="34" spans="13:16">
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
     </row>
     <row r="35" spans="13:16">
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
     </row>
     <row r="36" spans="13:16">
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
     </row>
     <row r="37" spans="13:16">
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
     </row>
     <row r="38" spans="13:16">
       <c r="N38"/>
@@ -2210,255 +2185,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H18"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="20">
-        <v>1.75</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="20">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="21">
-        <v>5</v>
-      </c>
-      <c r="H3" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="20">
-        <f>C2*C3</f>
-        <v>1.75</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="22">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="20">
-        <v>3</v>
-      </c>
-      <c r="H5" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="F6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="20">
-        <v>3</v>
-      </c>
-      <c r="H6" s="20">
-        <f>H4/C4</f>
-        <v>85.714285714285708</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="20">
-        <v>3</v>
-      </c>
-      <c r="H7" s="20">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="F9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="10">
-        <f>(RIGHT(F9,LEN(F9)-5)* $C$4) * $G$3</f>
-        <v>875</v>
-      </c>
-      <c r="H9" s="10">
-        <f>(RIGHT(F9,LEN(F9)-5)* $C$4) * $H$3</f>
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="10">
-        <f>(RIGHT(F10,LEN(F10)-5)* $C$4) * $G$3</f>
-        <v>787.5</v>
-      </c>
-      <c r="H10" s="10">
-        <f t="shared" ref="H10:H18" si="0">(RIGHT(F10,LEN(F10)-5)* $C$4) * $H$3</f>
-        <v>157.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="F11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" s="10">
-        <f t="shared" ref="G11:G18" si="1">(RIGHT(F11,LEN(F11)-5)* $C$4) * $G$3</f>
-        <v>700</v>
-      </c>
-      <c r="H11" s="10">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="F12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="10">
-        <f t="shared" si="1"/>
-        <v>612.5</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" si="0"/>
-        <v>122.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="10">
-        <f t="shared" si="1"/>
-        <v>525</v>
-      </c>
-      <c r="H13" s="10">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="10">
-        <f t="shared" si="1"/>
-        <v>437.5</v>
-      </c>
-      <c r="H14" s="10">
-        <f t="shared" si="0"/>
-        <v>87.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="F15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="10">
-        <f t="shared" si="1"/>
-        <v>350</v>
-      </c>
-      <c r="H15" s="10">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="F16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="10">
-        <f t="shared" si="1"/>
-        <v>262.5</v>
-      </c>
-      <c r="H16" s="10">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
-      </c>
-    </row>
-    <row r="17" spans="6:8">
-      <c r="F17" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="10">
-        <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="H17" s="10">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="6:8">
-      <c r="F18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="10">
-        <f t="shared" si="1"/>
-        <v>87.5</v>
-      </c>
-      <c r="H18" s="10">
-        <f t="shared" si="0"/>
-        <v>17.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>